<commit_message>
add 2 advance search
.....................
</commit_message>
<xml_diff>
--- a/how_to_use.xlsx
+++ b/how_to_use.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="111">
   <si>
     <t>parameter:</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -403,6 +403,28 @@
   </si>
   <si>
     <t>http://localhost/fyp_connect/driver_get_order_time.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>advance_search_food</t>
+  </si>
+  <si>
+    <t>advance_search_restaurant</t>
+  </si>
+  <si>
+    <t>keyword, type, min, max</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>keyword, type, district</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://localhost/fyp_connect/advance_search_food.php?keyword=tea&amp;type=Drink&amp;min=1&amp;max=15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://localhost/fyp_connect/advance_search_restaurant.php?keyword=tea&amp;type=Itailan&amp;district=Tai%20po</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -834,10 +856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5" x14ac:dyDescent="0.25"/>
@@ -864,13 +886,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>105</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>44</v>
+        <v>107</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -878,13 +900,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>106</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>45</v>
+        <v>108</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -892,548 +914,578 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>71</v>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>94</v>
+      <c r="C7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="7"/>
+      <c r="C8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="7"/>
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>47</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>48</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="7"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>89</v>
+        <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>90</v>
+        <v>29</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>100</v>
+        <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>103</v>
+        <v>30</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>104</v>
+        <v>90</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>95</v>
+        <v>102</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>78</v>
+        <v>13</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>76</v>
+        <v>14</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>73</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>49</v>
+        <v>16</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>50</v>
+        <v>17</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>97</v>
+        <v>14</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>99</v>
+        <v>32</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>16</v>
+        <v>97</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>58</v>
+        <v>98</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
+        <v>26</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D29" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
+        <v>28</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>29</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>30</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D33" s="5" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>31</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>32</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
+        <v>31</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>32</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>33</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D36" s="5" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>34</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>35</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>36</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>69</v>
+        <v>34</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>37</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>43</v>
+        <v>35</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>38</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>88</v>
+        <v>36</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
+        <v>37</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>38</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
         <v>39</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D42" s="5" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D40" r:id="rId1"/>
-    <hyperlink ref="D38" r:id="rId2"/>
-    <hyperlink ref="D2" r:id="rId3"/>
-    <hyperlink ref="D3" r:id="rId4"/>
-    <hyperlink ref="D6" r:id="rId5"/>
-    <hyperlink ref="D10" r:id="rId6"/>
-    <hyperlink ref="D11" r:id="rId7"/>
-    <hyperlink ref="D19" r:id="rId8"/>
-    <hyperlink ref="D20" r:id="rId9"/>
-    <hyperlink ref="D21" r:id="rId10"/>
-    <hyperlink ref="D22" r:id="rId11"/>
-    <hyperlink ref="D23" r:id="rId12"/>
-    <hyperlink ref="D26" r:id="rId13"/>
-    <hyperlink ref="D28" r:id="rId14"/>
-    <hyperlink ref="D31" r:id="rId15"/>
-    <hyperlink ref="D30" r:id="rId16"/>
-    <hyperlink ref="D27" r:id="rId17"/>
-    <hyperlink ref="D32" r:id="rId18"/>
-    <hyperlink ref="D34" r:id="rId19"/>
-    <hyperlink ref="D4" r:id="rId20"/>
-    <hyperlink ref="D24" r:id="rId21"/>
-    <hyperlink ref="D37" r:id="rId22"/>
-    <hyperlink ref="D5" r:id="rId23"/>
-    <hyperlink ref="D17" r:id="rId24"/>
-    <hyperlink ref="D18" r:id="rId25"/>
-    <hyperlink ref="D16" r:id="rId26"/>
-    <hyperlink ref="D36" r:id="rId27"/>
-    <hyperlink ref="D33" r:id="rId28"/>
-    <hyperlink ref="D7" r:id="rId29"/>
-    <hyperlink ref="D25" r:id="rId30"/>
-    <hyperlink ref="D13" r:id="rId31"/>
-    <hyperlink ref="D14" r:id="rId32"/>
+    <hyperlink ref="D42" r:id="rId1"/>
+    <hyperlink ref="D40" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D8" r:id="rId5"/>
+    <hyperlink ref="D12" r:id="rId6"/>
+    <hyperlink ref="D13" r:id="rId7"/>
+    <hyperlink ref="D21" r:id="rId8"/>
+    <hyperlink ref="D22" r:id="rId9"/>
+    <hyperlink ref="D23" r:id="rId10"/>
+    <hyperlink ref="D24" r:id="rId11"/>
+    <hyperlink ref="D25" r:id="rId12"/>
+    <hyperlink ref="D28" r:id="rId13"/>
+    <hyperlink ref="D30" r:id="rId14"/>
+    <hyperlink ref="D33" r:id="rId15"/>
+    <hyperlink ref="D32" r:id="rId16"/>
+    <hyperlink ref="D29" r:id="rId17"/>
+    <hyperlink ref="D34" r:id="rId18"/>
+    <hyperlink ref="D36" r:id="rId19"/>
+    <hyperlink ref="D6" r:id="rId20"/>
+    <hyperlink ref="D26" r:id="rId21"/>
+    <hyperlink ref="D39" r:id="rId22"/>
+    <hyperlink ref="D7" r:id="rId23"/>
+    <hyperlink ref="D19" r:id="rId24"/>
+    <hyperlink ref="D20" r:id="rId25"/>
+    <hyperlink ref="D18" r:id="rId26"/>
+    <hyperlink ref="D38" r:id="rId27"/>
+    <hyperlink ref="D35" r:id="rId28"/>
+    <hyperlink ref="D9" r:id="rId29"/>
+    <hyperlink ref="D27" r:id="rId30"/>
+    <hyperlink ref="D15" r:id="rId31"/>
+    <hyperlink ref="D16" r:id="rId32"/>
+    <hyperlink ref="D2" r:id="rId33"/>
+    <hyperlink ref="D3" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId33"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId35"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add order count rest
add order count rest
</commit_message>
<xml_diff>
--- a/how_to_use.xlsx
+++ b/how_to_use.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="120">
   <si>
     <t>parameter:</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -426,6 +426,40 @@
   <si>
     <t>http://localhost/fyp_connect/advance_search_restaurant.php?keyword=tea&amp;type=Itailan&amp;district=Tai%20po</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>driver_get_order2_qty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>driver_get_order2_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://localhost/fyp_connect/driver_get_order2_qty.php?id=d0001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://localhost/fyp_connect/driver_get_order2_time.php?id=d0001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get_order_rest_count</t>
+  </si>
+  <si>
+    <t>number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://localhost/fyp_connect/get_order_rest_count.php?number=1</t>
   </si>
 </sst>
 </file>
@@ -856,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5" x14ac:dyDescent="0.25"/>
@@ -925,7 +959,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
@@ -939,7 +973,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
@@ -953,7 +987,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
@@ -967,7 +1001,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
@@ -981,7 +1015,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>92</v>
@@ -995,7 +1029,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>24</v>
@@ -1005,7 +1039,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>25</v>
@@ -1015,7 +1049,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>8</v>
@@ -1029,7 +1063,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
@@ -1043,7 +1077,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>89</v>
@@ -1057,7 +1091,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>100</v>
@@ -1071,7 +1105,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>101</v>
@@ -1085,7 +1119,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>96</v>
@@ -1099,393 +1133,437 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>15</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>78</v>
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>16</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>76</v>
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>73</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>18</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>49</v>
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>19</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>50</v>
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>97</v>
+        <v>14</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>99</v>
+        <v>32</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>16</v>
+        <v>97</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>58</v>
+        <v>98</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>55</v>
+        <v>33</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>59</v>
+        <v>117</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>60</v>
+        <v>118</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D36" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>31</v>
-      </c>
-      <c r="B34" s="1" t="s">
+    <row r="37" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D37" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>32</v>
-      </c>
-      <c r="B35" s="1" t="s">
+    <row r="38" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D38" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>33</v>
-      </c>
-      <c r="B36" s="1" t="s">
+    <row r="39" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D39" s="5" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>34</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>35</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>36</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>43</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>38</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>88</v>
+        <v>40</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>39</v>
-      </c>
-      <c r="B42" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D45" s="5" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D42" r:id="rId1"/>
-    <hyperlink ref="D40" r:id="rId2"/>
+    <hyperlink ref="D45" r:id="rId1"/>
+    <hyperlink ref="D43" r:id="rId2"/>
     <hyperlink ref="D4" r:id="rId3"/>
     <hyperlink ref="D5" r:id="rId4"/>
     <hyperlink ref="D8" r:id="rId5"/>
     <hyperlink ref="D12" r:id="rId6"/>
     <hyperlink ref="D13" r:id="rId7"/>
-    <hyperlink ref="D21" r:id="rId8"/>
-    <hyperlink ref="D22" r:id="rId9"/>
-    <hyperlink ref="D23" r:id="rId10"/>
-    <hyperlink ref="D24" r:id="rId11"/>
-    <hyperlink ref="D25" r:id="rId12"/>
-    <hyperlink ref="D28" r:id="rId13"/>
-    <hyperlink ref="D30" r:id="rId14"/>
-    <hyperlink ref="D33" r:id="rId15"/>
-    <hyperlink ref="D32" r:id="rId16"/>
-    <hyperlink ref="D29" r:id="rId17"/>
-    <hyperlink ref="D34" r:id="rId18"/>
-    <hyperlink ref="D36" r:id="rId19"/>
+    <hyperlink ref="D23" r:id="rId8"/>
+    <hyperlink ref="D24" r:id="rId9"/>
+    <hyperlink ref="D25" r:id="rId10"/>
+    <hyperlink ref="D26" r:id="rId11"/>
+    <hyperlink ref="D27" r:id="rId12"/>
+    <hyperlink ref="D30" r:id="rId13"/>
+    <hyperlink ref="D33" r:id="rId14"/>
+    <hyperlink ref="D36" r:id="rId15"/>
+    <hyperlink ref="D35" r:id="rId16"/>
+    <hyperlink ref="D32" r:id="rId17"/>
+    <hyperlink ref="D37" r:id="rId18"/>
+    <hyperlink ref="D39" r:id="rId19"/>
     <hyperlink ref="D6" r:id="rId20"/>
-    <hyperlink ref="D26" r:id="rId21"/>
-    <hyperlink ref="D39" r:id="rId22"/>
+    <hyperlink ref="D28" r:id="rId21"/>
+    <hyperlink ref="D42" r:id="rId22"/>
     <hyperlink ref="D7" r:id="rId23"/>
-    <hyperlink ref="D19" r:id="rId24"/>
-    <hyperlink ref="D20" r:id="rId25"/>
-    <hyperlink ref="D18" r:id="rId26"/>
-    <hyperlink ref="D38" r:id="rId27"/>
-    <hyperlink ref="D35" r:id="rId28"/>
+    <hyperlink ref="D21" r:id="rId24"/>
+    <hyperlink ref="D22" r:id="rId25"/>
+    <hyperlink ref="D20" r:id="rId26"/>
+    <hyperlink ref="D41" r:id="rId27"/>
+    <hyperlink ref="D38" r:id="rId28"/>
     <hyperlink ref="D9" r:id="rId29"/>
-    <hyperlink ref="D27" r:id="rId30"/>
+    <hyperlink ref="D29" r:id="rId30"/>
     <hyperlink ref="D15" r:id="rId31"/>
     <hyperlink ref="D16" r:id="rId32"/>
     <hyperlink ref="D2" r:id="rId33"/>
     <hyperlink ref="D3" r:id="rId34"/>
+    <hyperlink ref="D18" r:id="rId35"/>
+    <hyperlink ref="D19" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId35"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId37"/>
 </worksheet>
 </file>
</xml_diff>